<commit_message>
#4 Fixed bug doesn't work when list in bean is defined
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/data/value/table/TestBook_definitionList.xlsx
+++ b/src/test/resources/org/xlbean/data/value/table/TestBook_definitionList.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\src\test\resources\org\xlbean\reader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\src\test\resources\org\xlbean\data\value\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A053BD61-6AE3-4D1C-B47B-344B29F00539}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8397CE8-225C-4F8D-9DD1-7126DE32A0E4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="format" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>####</t>
     <phoneticPr fontId="1"/>
@@ -121,6 +122,16 @@
   <si>
     <t>deflist#value?listToPropValue=true</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>obj.deflist#key?listToPropKey=true</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>obj.deflist#value?listToPropValue=true</t>
+  </si>
+  <si>
+    <t>obj.deflist#~</t>
   </si>
 </sst>
 </file>
@@ -700,9 +711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -985,4 +994,292 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2861CD42-422C-47FA-9E5A-3F259455E206}">
+  <dimension ref="A1:AA23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.25" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.08203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.25" customWidth="1"/>
+    <col min="14" max="14" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.08203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="16" customWidth="1"/>
+    <col min="24" max="24" width="6.83203125" customWidth="1"/>
+    <col min="25" max="25" width="19.33203125" customWidth="1"/>
+    <col min="27" max="27" width="6.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>12345</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="53"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="X3" s="27"/>
+      <c r="AA3" s="27"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="N4" s="1"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="Y4" s="44"/>
+      <c r="Z4" s="2"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="49"/>
+      <c r="G5" s="28"/>
+      <c r="J5" s="35"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="38"/>
+      <c r="S5" s="43"/>
+      <c r="T5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="Y5" s="45"/>
+      <c r="Z5" s="2"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="50"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="J6" s="36"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="3"/>
+      <c r="Y6" s="46"/>
+      <c r="Z6" s="2"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39"/>
+      <c r="Y7" s="47"/>
+      <c r="Z7" s="2"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="20"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="Y8" s="48"/>
+      <c r="Z8" s="2"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="22"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="23"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="42"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="25"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="38"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="37"/>
+    </row>
+    <row r="17" spans="13:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+    </row>
+    <row r="18" spans="13:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="37"/>
+    </row>
+    <row r="19" spans="13:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+    </row>
+    <row r="20" spans="13:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+    </row>
+    <row r="21" spans="13:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+    </row>
+    <row r="22" spans="13:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+    </row>
+    <row r="23" spans="13:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#10 Changed property name to listToProp=key and listToProp=value
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/data/value/table/TestBook_definitionList.xlsx
+++ b/src/test/resources/org/xlbean/data/value/table/TestBook_definitionList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\src\test\resources\org\xlbean\data\value\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8397CE8-225C-4F8D-9DD1-7126DE32A0E4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6387452-3B2A-4CAB-A7CE-767F969A59E3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,22 +116,23 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>deflist#key?listToPropKey=true</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>deflist#value?listToPropValue=true</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>obj.deflist#key?listToPropKey=true</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>obj.deflist#value?listToPropValue=true</t>
-  </si>
-  <si>
     <t>obj.deflist#~</t>
+  </si>
+  <si>
+    <t>obj.deflist#key?listToProp=key</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>obj.deflist#value?listToProp=value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>deflist#key?listToProp=key</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>deflist#value?listToProp=value</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -711,7 +712,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -747,10 +750,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.55000000000000004">
@@ -1000,7 +1003,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2861CD42-422C-47FA-9E5A-3F259455E206}">
   <dimension ref="A1:AA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1036,15 +1041,15 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>

</xml_diff>